<commit_message>
FEB 4th Plan updated
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="24000" windowHeight="8985" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="24000" windowHeight="8985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts to Cover" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="237">
   <si>
     <t>Design Patterns</t>
   </si>
@@ -2203,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,9 +2266,15 @@
       <c r="A4" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -2791,7 +2797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Concurrency Learning link added in first page
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t7959ak\Desktop\Raman\JavaLearning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GSR\JAP\Code\GIT Extensions\NewRep\JavaLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="24000" windowHeight="8985" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="24000" windowHeight="8985"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts to Cover" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="238">
   <si>
     <t>Design Patterns</t>
   </si>
@@ -741,6 +741,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>http://tutorials.jenkov.com/java-concurrency/concurrency-models.html</t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,6 +1145,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2791,7 +2797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Feb 4th week plan updated
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GSR\JAP\Code\GIT Extensions\NewRep\JavaLearning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t7959ak\Desktop\Raman\JavaLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="24000" windowHeight="8985"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="24000" windowHeight="8985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts to Cover" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="238">
   <si>
     <t>Design Patterns</t>
   </si>
@@ -1127,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2209,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,9 +2272,15 @@
       <c r="A4" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>

</xml_diff>